<commit_message>
moana prog odciecia 82
</commit_message>
<xml_diff>
--- a/SourceCode/efficientnet_pytorch/PixelHeatMap.xlsx
+++ b/SourceCode/efficientnet_pytorch/PixelHeatMap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27960" windowHeight="12600" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27960" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="windowRatioCalculation" sheetId="5" r:id="rId1"/>
@@ -7372,10 +7372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7436,30 +7436,30 @@
         <v>60</v>
       </c>
       <c r="F2" s="28">
-        <v>960</v>
+        <v>420</v>
       </c>
       <c r="G2" s="29">
-        <v>540</v>
+        <v>330</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="J2" s="30">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="K2" s="28">
-        <v>1016</v>
+        <v>420</v>
       </c>
       <c r="L2" s="29">
-        <v>573</v>
+        <v>330</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="O2" s="30">
-        <v>150</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15">
@@ -7522,22 +7522,22 @@
       <c r="E5" s="30"/>
       <c r="F5" s="28">
         <f>ROUNDDOWN((F2-I2)/J2+1,0)</f>
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G5" s="28">
         <f>ROUNDDOWN((G2-I2)/J2+1,0)</f>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="30"/>
       <c r="K5" s="28">
         <f>ROUNDDOWN((K2-N2)/O2+1,0)</f>
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L5" s="28">
         <f>ROUNDDOWN((L2-N2)/O2+1,0)</f>
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="M5" s="29"/>
       <c r="N5" s="29"/>
@@ -7578,7 +7578,7 @@
       <c r="F7" s="28"/>
       <c r="G7" s="29">
         <f>F5*G5</f>
-        <v>480</v>
+        <v>1598</v>
       </c>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -7586,7 +7586,7 @@
       <c r="K7" s="28"/>
       <c r="L7" s="29">
         <f>K5*L5</f>
-        <v>18</v>
+        <v>1189</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
@@ -7678,12 +7678,12 @@
       </c>
       <c r="G11" s="31">
         <f>G2/F2*F11</f>
-        <v>576</v>
+        <v>804.57142857142856</v>
       </c>
       <c r="H11" s="31"/>
       <c r="I11" s="31">
         <f>F11/F2</f>
-        <v>1.0666666666666667</v>
+        <v>2.4380952380952383</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="10">
@@ -7691,12 +7691,12 @@
       </c>
       <c r="L11" s="31">
         <f>L2/K2*K11</f>
-        <v>577.51181102362204</v>
+        <v>804.57142857142856</v>
       </c>
       <c r="M11" s="31"/>
       <c r="N11" s="31">
         <f>K11/K2</f>
-        <v>1.0078740157480315</v>
+        <v>2.4380952380952383</v>
       </c>
       <c r="O11" s="12"/>
     </row>
@@ -7765,22 +7765,22 @@
       <c r="E15" s="12"/>
       <c r="F15" s="10">
         <f>F11/I11</f>
-        <v>960</v>
+        <v>419.99999999999994</v>
       </c>
       <c r="G15" s="31">
         <f>G11/I11</f>
-        <v>540</v>
+        <v>329.99999999999994</v>
       </c>
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
       <c r="J15" s="12"/>
       <c r="K15" s="10">
         <f>K11/N11</f>
-        <v>1016</v>
+        <v>419.99999999999994</v>
       </c>
       <c r="L15" s="31">
         <f>L11/N11</f>
-        <v>573</v>
+        <v>329.99999999999994</v>
       </c>
       <c r="M15" s="31"/>
       <c r="N15" s="31"/>
@@ -7920,6 +7920,16 @@
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
       <c r="O21" s="15"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35">
+        <v>420</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45617,7 +45627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>

</xml_diff>